<commit_message>
bash script and new results for COVID scenario
</commit_message>
<xml_diff>
--- a/Somalia-COVID-impact/Results_COVID_Cholera_National.xlsx
+++ b/Somalia-COVID-impact/Results_COVID_Cholera_National.xlsx
@@ -7,7 +7,7 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="National" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -483,16 +483,16 @@
         <v>1</v>
       </c>
       <c r="B3" t="n">
-        <v>97.93000000000001</v>
+        <v>97.84</v>
       </c>
       <c r="C3" t="n">
-        <v>0.76</v>
+        <v>0.85</v>
       </c>
       <c r="D3" t="n">
-        <v>1.01</v>
+        <v>1.02</v>
       </c>
       <c r="E3" t="n">
-        <v>0.14</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="4">
@@ -500,16 +500,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="n">
-        <v>97.98999999999999</v>
+        <v>97.88</v>
       </c>
       <c r="C4" t="n">
-        <v>0.71</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="D4" t="n">
-        <v>1.02</v>
+        <v>1.03</v>
       </c>
       <c r="E4" t="n">
-        <v>0.13</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="5">
@@ -517,16 +517,16 @@
         <v>3</v>
       </c>
       <c r="B5" t="n">
-        <v>98.06</v>
+        <v>97.93000000000001</v>
       </c>
       <c r="C5" t="n">
-        <v>0.66</v>
+        <v>0.76</v>
       </c>
       <c r="D5" t="n">
-        <v>1.02</v>
+        <v>1.04</v>
       </c>
       <c r="E5" t="n">
-        <v>0.12</v>
+        <v>0.19</v>
       </c>
     </row>
     <row r="6">
@@ -534,16 +534,16 @@
         <v>4</v>
       </c>
       <c r="B6" t="n">
-        <v>98.12</v>
+        <v>97.98</v>
       </c>
       <c r="C6" t="n">
-        <v>0.61</v>
+        <v>0.73</v>
       </c>
       <c r="D6" t="n">
-        <v>1.01</v>
+        <v>1.04</v>
       </c>
       <c r="E6" t="n">
-        <v>0.11</v>
+        <v>0.18</v>
       </c>
     </row>
     <row r="7">
@@ -551,16 +551,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="n">
-        <v>98.19</v>
+        <v>98.03</v>
       </c>
       <c r="C7" t="n">
-        <v>0.57</v>
+        <v>0.6899999999999999</v>
       </c>
       <c r="D7" t="n">
-        <v>1.01</v>
+        <v>1.04</v>
       </c>
       <c r="E7" t="n">
-        <v>0.11</v>
+        <v>0.17</v>
       </c>
     </row>
     <row r="8">
@@ -568,16 +568,16 @@
         <v>6</v>
       </c>
       <c r="B8" t="n">
-        <v>98.25</v>
+        <v>98.08</v>
       </c>
       <c r="C8" t="n">
-        <v>0.53</v>
+        <v>0.65</v>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
+        <v>1.04</v>
       </c>
       <c r="E8" t="n">
-        <v>0.1</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="9">
@@ -585,16 +585,16 @@
         <v>7</v>
       </c>
       <c r="B9" t="n">
-        <v>98.31999999999999</v>
+        <v>98.13</v>
       </c>
       <c r="C9" t="n">
-        <v>0.49</v>
+        <v>0.62</v>
       </c>
       <c r="D9" t="n">
-        <v>0.98</v>
+        <v>1.04</v>
       </c>
       <c r="E9" t="n">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
     </row>
     <row r="10">
@@ -602,16 +602,16 @@
         <v>8</v>
       </c>
       <c r="B10" t="n">
-        <v>98.38</v>
+        <v>98.19</v>
       </c>
       <c r="C10" t="n">
-        <v>0.46</v>
+        <v>0.59</v>
       </c>
       <c r="D10" t="n">
-        <v>0.97</v>
+        <v>1.03</v>
       </c>
       <c r="E10" t="n">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="11">
@@ -619,16 +619,16 @@
         <v>9</v>
       </c>
       <c r="B11" t="n">
-        <v>98.44</v>
+        <v>98.23999999999999</v>
       </c>
       <c r="C11" t="n">
-        <v>0.43</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="D11" t="n">
-        <v>0.95</v>
+        <v>1.02</v>
       </c>
       <c r="E11" t="n">
-        <v>0.08</v>
+        <v>0.14</v>
       </c>
     </row>
     <row r="12">
@@ -636,16 +636,16 @@
         <v>10</v>
       </c>
       <c r="B12" t="n">
-        <v>98.5</v>
+        <v>98.29000000000001</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4</v>
+        <v>0.53</v>
       </c>
       <c r="D12" t="n">
-        <v>0.93</v>
+        <v>1.01</v>
       </c>
       <c r="E12" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="13">
@@ -653,16 +653,16 @@
         <v>11</v>
       </c>
       <c r="B13" t="n">
-        <v>98.56</v>
+        <v>98.34</v>
       </c>
       <c r="C13" t="n">
-        <v>0.37</v>
+        <v>0.51</v>
       </c>
       <c r="D13" t="n">
-        <v>0.91</v>
+        <v>0.99</v>
       </c>
       <c r="E13" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="14">
@@ -670,16 +670,16 @@
         <v>12</v>
       </c>
       <c r="B14" t="n">
-        <v>98.62</v>
+        <v>98.39</v>
       </c>
       <c r="C14" t="n">
-        <v>0.34</v>
+        <v>0.48</v>
       </c>
       <c r="D14" t="n">
-        <v>0.89</v>
+        <v>0.98</v>
       </c>
       <c r="E14" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
     </row>
     <row r="15">
@@ -687,16 +687,16 @@
         <v>13</v>
       </c>
       <c r="B15" t="n">
-        <v>98.67</v>
+        <v>98.44</v>
       </c>
       <c r="C15" t="n">
-        <v>0.32</v>
+        <v>0.46</v>
       </c>
       <c r="D15" t="n">
-        <v>0.86</v>
+        <v>0.96</v>
       </c>
       <c r="E15" t="n">
-        <v>0.06</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="16">
@@ -704,16 +704,16 @@
         <v>14</v>
       </c>
       <c r="B16" t="n">
-        <v>98.72</v>
+        <v>98.48999999999999</v>
       </c>
       <c r="C16" t="n">
-        <v>0.3</v>
+        <v>0.43</v>
       </c>
       <c r="D16" t="n">
-        <v>0.84</v>
+        <v>0.95</v>
       </c>
       <c r="E16" t="n">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="17">
@@ -721,16 +721,16 @@
         <v>15</v>
       </c>
       <c r="B17" t="n">
-        <v>98.78</v>
+        <v>98.53</v>
       </c>
       <c r="C17" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="D17" t="n">
-        <v>0.82</v>
+        <v>0.93</v>
       </c>
       <c r="E17" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="18">
@@ -738,16 +738,16 @@
         <v>16</v>
       </c>
       <c r="B18" t="n">
-        <v>98.83</v>
+        <v>98.58</v>
       </c>
       <c r="C18" t="n">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="D18" t="n">
-        <v>0.79</v>
+        <v>0.91</v>
       </c>
       <c r="E18" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="19">
@@ -755,16 +755,16 @@
         <v>17</v>
       </c>
       <c r="B19" t="n">
-        <v>98.88</v>
+        <v>98.63</v>
       </c>
       <c r="C19" t="n">
-        <v>0.24</v>
+        <v>0.37</v>
       </c>
       <c r="D19" t="n">
-        <v>0.77</v>
+        <v>0.89</v>
       </c>
       <c r="E19" t="n">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="20">
@@ -772,16 +772,16 @@
         <v>18</v>
       </c>
       <c r="B20" t="n">
-        <v>98.93000000000001</v>
+        <v>98.67</v>
       </c>
       <c r="C20" t="n">
-        <v>0.22</v>
+        <v>0.35</v>
       </c>
       <c r="D20" t="n">
-        <v>0.74</v>
+        <v>0.87</v>
       </c>
       <c r="E20" t="n">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="21">
@@ -789,16 +789,16 @@
         <v>19</v>
       </c>
       <c r="B21" t="n">
-        <v>98.97</v>
+        <v>98.72</v>
       </c>
       <c r="C21" t="n">
-        <v>0.21</v>
+        <v>0.33</v>
       </c>
       <c r="D21" t="n">
-        <v>0.72</v>
+        <v>0.85</v>
       </c>
       <c r="E21" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="22">
@@ -806,16 +806,16 @@
         <v>20</v>
       </c>
       <c r="B22" t="n">
-        <v>99.02</v>
+        <v>98.76000000000001</v>
       </c>
       <c r="C22" t="n">
-        <v>0.19</v>
+        <v>0.32</v>
       </c>
       <c r="D22" t="n">
-        <v>0.6899999999999999</v>
+        <v>0.83</v>
       </c>
       <c r="E22" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="23">
@@ -823,16 +823,16 @@
         <v>21</v>
       </c>
       <c r="B23" t="n">
-        <v>99.06</v>
+        <v>98.8</v>
       </c>
       <c r="C23" t="n">
-        <v>0.18</v>
+        <v>0.3</v>
       </c>
       <c r="D23" t="n">
-        <v>0.67</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="E23" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
     </row>
     <row r="24">
@@ -840,16 +840,16 @@
         <v>22</v>
       </c>
       <c r="B24" t="n">
-        <v>99.09999999999999</v>
+        <v>98.84</v>
       </c>
       <c r="C24" t="n">
-        <v>0.17</v>
+        <v>0.29</v>
       </c>
       <c r="D24" t="n">
-        <v>0.65</v>
+        <v>0.78</v>
       </c>
       <c r="E24" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="25">
@@ -857,16 +857,16 @@
         <v>23</v>
       </c>
       <c r="B25" t="n">
-        <v>99.14</v>
+        <v>98.88</v>
       </c>
       <c r="C25" t="n">
-        <v>0.16</v>
+        <v>0.27</v>
       </c>
       <c r="D25" t="n">
-        <v>0.62</v>
+        <v>0.76</v>
       </c>
       <c r="E25" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="26">
@@ -874,16 +874,16 @@
         <v>24</v>
       </c>
       <c r="B26" t="n">
-        <v>99.18000000000001</v>
+        <v>98.92</v>
       </c>
       <c r="C26" t="n">
-        <v>0.15</v>
+        <v>0.26</v>
       </c>
       <c r="D26" t="n">
-        <v>0.6</v>
+        <v>0.74</v>
       </c>
       <c r="E26" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
     </row>
     <row r="27">
@@ -891,16 +891,16 @@
         <v>25</v>
       </c>
       <c r="B27" t="n">
-        <v>99.22</v>
+        <v>98.95999999999999</v>
       </c>
       <c r="C27" t="n">
-        <v>0.13</v>
+        <v>0.25</v>
       </c>
       <c r="D27" t="n">
-        <v>0.58</v>
+        <v>0.72</v>
       </c>
       <c r="E27" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="28">
@@ -908,16 +908,16 @@
         <v>26</v>
       </c>
       <c r="B28" t="n">
-        <v>99.25</v>
+        <v>99</v>
       </c>
       <c r="C28" t="n">
-        <v>0.13</v>
+        <v>0.23</v>
       </c>
       <c r="D28" t="n">
-        <v>0.5600000000000001</v>
+        <v>0.7</v>
       </c>
       <c r="E28" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="29">
@@ -925,16 +925,16 @@
         <v>27</v>
       </c>
       <c r="B29" t="n">
-        <v>99.29000000000001</v>
+        <v>99.04000000000001</v>
       </c>
       <c r="C29" t="n">
-        <v>0.12</v>
+        <v>0.22</v>
       </c>
       <c r="D29" t="n">
-        <v>0.53</v>
+        <v>0.68</v>
       </c>
       <c r="E29" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
     </row>
     <row r="30">
@@ -942,16 +942,16 @@
         <v>28</v>
       </c>
       <c r="B30" t="n">
-        <v>99.31999999999999</v>
+        <v>99.06999999999999</v>
       </c>
       <c r="C30" t="n">
-        <v>0.11</v>
+        <v>0.21</v>
       </c>
       <c r="D30" t="n">
-        <v>0.51</v>
+        <v>0.66</v>
       </c>
       <c r="E30" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="31">
@@ -959,16 +959,16 @@
         <v>29</v>
       </c>
       <c r="B31" t="n">
-        <v>99.34999999999999</v>
+        <v>99.11</v>
       </c>
       <c r="C31" t="n">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="D31" t="n">
-        <v>0.49</v>
+        <v>0.64</v>
       </c>
       <c r="E31" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="32">
@@ -976,16 +976,16 @@
         <v>30</v>
       </c>
       <c r="B32" t="n">
-        <v>99.38</v>
+        <v>99.14</v>
       </c>
       <c r="C32" t="n">
-        <v>0.09</v>
+        <v>0.19</v>
       </c>
       <c r="D32" t="n">
-        <v>0.47</v>
+        <v>0.62</v>
       </c>
       <c r="E32" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="33">
@@ -993,16 +993,16 @@
         <v>31</v>
       </c>
       <c r="B33" t="n">
-        <v>99.41</v>
+        <v>99.17</v>
       </c>
       <c r="C33" t="n">
-        <v>0.09</v>
+        <v>0.18</v>
       </c>
       <c r="D33" t="n">
-        <v>0.45</v>
+        <v>0.6</v>
       </c>
       <c r="E33" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="34">
@@ -1010,16 +1010,16 @@
         <v>32</v>
       </c>
       <c r="B34" t="n">
-        <v>99.44</v>
+        <v>99.2</v>
       </c>
       <c r="C34" t="n">
-        <v>0.08</v>
+        <v>0.17</v>
       </c>
       <c r="D34" t="n">
-        <v>0.43</v>
+        <v>0.58</v>
       </c>
       <c r="E34" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="35">
@@ -1027,16 +1027,16 @@
         <v>33</v>
       </c>
       <c r="B35" t="n">
-        <v>99.47</v>
+        <v>99.23</v>
       </c>
       <c r="C35" t="n">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="D35" t="n">
-        <v>0.41</v>
+        <v>0.5600000000000001</v>
       </c>
       <c r="E35" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="36">
@@ -1044,16 +1044,16 @@
         <v>34</v>
       </c>
       <c r="B36" t="n">
-        <v>99.48999999999999</v>
+        <v>99.26000000000001</v>
       </c>
       <c r="C36" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.16</v>
       </c>
       <c r="D36" t="n">
-        <v>0.4</v>
+        <v>0.54</v>
       </c>
       <c r="E36" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="37">
@@ -1061,16 +1061,16 @@
         <v>35</v>
       </c>
       <c r="B37" t="n">
-        <v>99.52</v>
+        <v>99.29000000000001</v>
       </c>
       <c r="C37" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.15</v>
       </c>
       <c r="D37" t="n">
-        <v>0.38</v>
+        <v>0.52</v>
       </c>
       <c r="E37" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="38">
@@ -1078,16 +1078,16 @@
         <v>36</v>
       </c>
       <c r="B38" t="n">
-        <v>99.54000000000001</v>
+        <v>99.31999999999999</v>
       </c>
       <c r="C38" t="n">
-        <v>0.06</v>
+        <v>0.14</v>
       </c>
       <c r="D38" t="n">
-        <v>0.36</v>
+        <v>0.51</v>
       </c>
       <c r="E38" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="39">
@@ -1095,16 +1095,16 @@
         <v>37</v>
       </c>
       <c r="B39" t="n">
-        <v>99.56</v>
+        <v>99.34</v>
       </c>
       <c r="C39" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="D39" t="n">
-        <v>0.35</v>
+        <v>0.49</v>
       </c>
       <c r="E39" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="40">
@@ -1112,16 +1112,16 @@
         <v>38</v>
       </c>
       <c r="B40" t="n">
-        <v>99.58</v>
+        <v>99.37</v>
       </c>
       <c r="C40" t="n">
-        <v>0.05</v>
+        <v>0.13</v>
       </c>
       <c r="D40" t="n">
-        <v>0.33</v>
+        <v>0.47</v>
       </c>
       <c r="E40" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="41">
@@ -1129,16 +1129,16 @@
         <v>39</v>
       </c>
       <c r="B41" t="n">
-        <v>99.59999999999999</v>
+        <v>99.39</v>
       </c>
       <c r="C41" t="n">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="D41" t="n">
-        <v>0.32</v>
+        <v>0.45</v>
       </c>
       <c r="E41" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="42">
@@ -1146,16 +1146,16 @@
         <v>40</v>
       </c>
       <c r="B42" t="n">
-        <v>99.62</v>
+        <v>99.42</v>
       </c>
       <c r="C42" t="n">
-        <v>0.05</v>
+        <v>0.12</v>
       </c>
       <c r="D42" t="n">
-        <v>0.3</v>
+        <v>0.44</v>
       </c>
       <c r="E42" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="43">
@@ -1163,16 +1163,16 @@
         <v>41</v>
       </c>
       <c r="B43" t="n">
-        <v>99.64</v>
+        <v>99.44</v>
       </c>
       <c r="C43" t="n">
-        <v>0.04</v>
+        <v>0.11</v>
       </c>
       <c r="D43" t="n">
-        <v>0.29</v>
+        <v>0.42</v>
       </c>
       <c r="E43" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="44">
@@ -1180,16 +1180,16 @@
         <v>42</v>
       </c>
       <c r="B44" t="n">
-        <v>99.66</v>
+        <v>99.45999999999999</v>
       </c>
       <c r="C44" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="D44" t="n">
-        <v>0.28</v>
+        <v>0.41</v>
       </c>
       <c r="E44" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
     </row>
     <row r="45">
@@ -1197,16 +1197,16 @@
         <v>43</v>
       </c>
       <c r="B45" t="n">
-        <v>99.68000000000001</v>
+        <v>99.48</v>
       </c>
       <c r="C45" t="n">
-        <v>0.04</v>
+        <v>0.1</v>
       </c>
       <c r="D45" t="n">
-        <v>0.26</v>
+        <v>0.39</v>
       </c>
       <c r="E45" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="46">
@@ -1214,16 +1214,16 @@
         <v>44</v>
       </c>
       <c r="B46" t="n">
-        <v>99.69</v>
+        <v>99.51000000000001</v>
       </c>
       <c r="C46" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="D46" t="n">
-        <v>0.25</v>
+        <v>0.38</v>
       </c>
       <c r="E46" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="47">
@@ -1231,16 +1231,16 @@
         <v>45</v>
       </c>
       <c r="B47" t="n">
-        <v>99.70999999999999</v>
+        <v>99.53</v>
       </c>
       <c r="C47" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="D47" t="n">
-        <v>0.24</v>
+        <v>0.36</v>
       </c>
       <c r="E47" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="48">
@@ -1248,16 +1248,16 @@
         <v>46</v>
       </c>
       <c r="B48" t="n">
-        <v>99.72</v>
+        <v>99.54000000000001</v>
       </c>
       <c r="C48" t="n">
-        <v>0.03</v>
+        <v>0.09</v>
       </c>
       <c r="D48" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="E48" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="49">
@@ -1265,16 +1265,16 @@
         <v>47</v>
       </c>
       <c r="B49" t="n">
-        <v>99.73999999999999</v>
+        <v>99.56</v>
       </c>
       <c r="C49" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="D49" t="n">
-        <v>0.22</v>
+        <v>0.34</v>
       </c>
       <c r="E49" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="50">
@@ -1282,16 +1282,16 @@
         <v>48</v>
       </c>
       <c r="B50" t="n">
-        <v>99.75</v>
+        <v>99.58</v>
       </c>
       <c r="C50" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="D50" t="n">
-        <v>0.21</v>
+        <v>0.32</v>
       </c>
       <c r="E50" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="51">
@@ -1299,16 +1299,16 @@
         <v>49</v>
       </c>
       <c r="B51" t="n">
-        <v>99.76000000000001</v>
+        <v>99.59999999999999</v>
       </c>
       <c r="C51" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D51" t="n">
+        <v>0.31</v>
+      </c>
+      <c r="E51" t="n">
         <v>0.02</v>
-      </c>
-      <c r="D51" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="E51" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1316,16 +1316,16 @@
         <v>50</v>
       </c>
       <c r="B52" t="n">
-        <v>99.77</v>
+        <v>99.61</v>
       </c>
       <c r="C52" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D52" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="E52" t="n">
         <v>0.02</v>
-      </c>
-      <c r="D52" t="n">
-        <v>0.19</v>
-      </c>
-      <c r="E52" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1333,16 +1333,16 @@
         <v>51</v>
       </c>
       <c r="B53" t="n">
-        <v>99.79000000000001</v>
+        <v>99.63</v>
       </c>
       <c r="C53" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="D53" t="n">
+        <v>0.29</v>
+      </c>
+      <c r="E53" t="n">
         <v>0.02</v>
-      </c>
-      <c r="D53" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="54">
@@ -1350,16 +1350,16 @@
         <v>52</v>
       </c>
       <c r="B54" t="n">
-        <v>99.8</v>
+        <v>99.65000000000001</v>
       </c>
       <c r="C54" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D54" t="n">
+        <v>0.28</v>
+      </c>
+      <c r="E54" t="n">
         <v>0.02</v>
-      </c>
-      <c r="D54" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="E54" t="n">
-        <v>0</v>
       </c>
     </row>
     <row r="55">
@@ -1367,16 +1367,16 @@
         <v>53</v>
       </c>
       <c r="B55" t="n">
-        <v>99.81</v>
+        <v>99.66</v>
       </c>
       <c r="C55" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="D55" t="n">
-        <v>0.16</v>
+        <v>0.27</v>
       </c>
       <c r="E55" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="56">
@@ -1384,16 +1384,16 @@
         <v>54</v>
       </c>
       <c r="B56" t="n">
-        <v>99.81999999999999</v>
+        <v>99.67</v>
       </c>
       <c r="C56" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="D56" t="n">
-        <v>0.15</v>
+        <v>0.26</v>
       </c>
       <c r="E56" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="57">
@@ -1401,16 +1401,16 @@
         <v>55</v>
       </c>
       <c r="B57" t="n">
-        <v>99.83</v>
+        <v>99.69</v>
       </c>
       <c r="C57" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="D57" t="n">
-        <v>0.15</v>
+        <v>0.25</v>
       </c>
       <c r="E57" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="58">
@@ -1418,16 +1418,16 @@
         <v>56</v>
       </c>
       <c r="B58" t="n">
-        <v>99.84</v>
+        <v>99.7</v>
       </c>
       <c r="C58" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D58" t="n">
-        <v>0.14</v>
+        <v>0.24</v>
       </c>
       <c r="E58" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="59">
@@ -1435,16 +1435,16 @@
         <v>57</v>
       </c>
       <c r="B59" t="n">
-        <v>99.84</v>
+        <v>99.70999999999999</v>
       </c>
       <c r="C59" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D59" t="n">
-        <v>0.13</v>
+        <v>0.23</v>
       </c>
       <c r="E59" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="60">
@@ -1452,16 +1452,16 @@
         <v>58</v>
       </c>
       <c r="B60" t="n">
-        <v>99.84999999999999</v>
+        <v>99.73</v>
       </c>
       <c r="C60" t="n">
-        <v>0.01</v>
+        <v>0.05</v>
       </c>
       <c r="D60" t="n">
-        <v>0.13</v>
+        <v>0.22</v>
       </c>
       <c r="E60" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="61">
@@ -1469,16 +1469,16 @@
         <v>59</v>
       </c>
       <c r="B61" t="n">
-        <v>99.86</v>
+        <v>99.73999999999999</v>
       </c>
       <c r="C61" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D61" t="n">
-        <v>0.12</v>
+        <v>0.21</v>
       </c>
       <c r="E61" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="62">
@@ -1486,16 +1486,16 @@
         <v>60</v>
       </c>
       <c r="B62" t="n">
-        <v>99.87</v>
+        <v>99.75</v>
       </c>
       <c r="C62" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D62" t="n">
-        <v>0.11</v>
+        <v>0.2</v>
       </c>
       <c r="E62" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="63">
@@ -1503,16 +1503,16 @@
         <v>61</v>
       </c>
       <c r="B63" t="n">
-        <v>99.87</v>
+        <v>99.76000000000001</v>
       </c>
       <c r="C63" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D63" t="n">
-        <v>0.11</v>
+        <v>0.19</v>
       </c>
       <c r="E63" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64">
@@ -1520,16 +1520,16 @@
         <v>62</v>
       </c>
       <c r="B64" t="n">
-        <v>99.88</v>
+        <v>99.77</v>
       </c>
       <c r="C64" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D64" t="n">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="E64" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="65">
@@ -1537,16 +1537,16 @@
         <v>63</v>
       </c>
       <c r="B65" t="n">
-        <v>99.89</v>
+        <v>99.78</v>
       </c>
       <c r="C65" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="D65" t="n">
-        <v>0.1</v>
+        <v>0.18</v>
       </c>
       <c r="E65" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="66">
@@ -1554,16 +1554,16 @@
         <v>64</v>
       </c>
       <c r="B66" t="n">
-        <v>99.89</v>
+        <v>99.79000000000001</v>
       </c>
       <c r="C66" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D66" t="n">
-        <v>0.09</v>
+        <v>0.17</v>
       </c>
       <c r="E66" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="67">
@@ -1571,16 +1571,16 @@
         <v>65</v>
       </c>
       <c r="B67" t="n">
-        <v>99.90000000000001</v>
+        <v>99.8</v>
       </c>
       <c r="C67" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D67" t="n">
-        <v>0.09</v>
+        <v>0.16</v>
       </c>
       <c r="E67" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="68">
@@ -1588,16 +1588,16 @@
         <v>66</v>
       </c>
       <c r="B68" t="n">
-        <v>99.90000000000001</v>
+        <v>99.81</v>
       </c>
       <c r="C68" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D68" t="n">
-        <v>0.08</v>
+        <v>0.16</v>
       </c>
       <c r="E68" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="69">
@@ -1605,16 +1605,16 @@
         <v>67</v>
       </c>
       <c r="B69" t="n">
-        <v>99.91</v>
+        <v>99.81</v>
       </c>
       <c r="C69" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D69" t="n">
-        <v>0.08</v>
+        <v>0.15</v>
       </c>
       <c r="E69" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="70">
@@ -1622,16 +1622,16 @@
         <v>68</v>
       </c>
       <c r="B70" t="n">
-        <v>99.91</v>
+        <v>99.81999999999999</v>
       </c>
       <c r="C70" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D70" t="n">
-        <v>0.08</v>
+        <v>0.14</v>
       </c>
       <c r="E70" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="71">
@@ -1639,16 +1639,16 @@
         <v>69</v>
       </c>
       <c r="B71" t="n">
-        <v>99.92</v>
+        <v>99.83</v>
       </c>
       <c r="C71" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D71" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.14</v>
       </c>
       <c r="E71" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="72">
@@ -1656,16 +1656,16 @@
         <v>70</v>
       </c>
       <c r="B72" t="n">
-        <v>99.92</v>
+        <v>99.84</v>
       </c>
       <c r="C72" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="D72" t="n">
-        <v>0.07000000000000001</v>
+        <v>0.13</v>
       </c>
       <c r="E72" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="73">
@@ -1673,16 +1673,16 @@
         <v>71</v>
       </c>
       <c r="B73" t="n">
-        <v>99.93000000000001</v>
+        <v>99.84</v>
       </c>
       <c r="C73" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="D73" t="n">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="E73" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="74">
@@ -1690,16 +1690,16 @@
         <v>72</v>
       </c>
       <c r="B74" t="n">
-        <v>99.93000000000001</v>
+        <v>99.84999999999999</v>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D74" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="E74" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="75">
@@ -1707,16 +1707,16 @@
         <v>73</v>
       </c>
       <c r="B75" t="n">
-        <v>99.93000000000001</v>
+        <v>99.86</v>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D75" t="n">
-        <v>0.06</v>
+        <v>0.12</v>
       </c>
       <c r="E75" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="76">
@@ -1724,16 +1724,16 @@
         <v>74</v>
       </c>
       <c r="B76" t="n">
-        <v>99.94</v>
+        <v>99.86</v>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D76" t="n">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="E76" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="77">
@@ -1741,16 +1741,16 @@
         <v>75</v>
       </c>
       <c r="B77" t="n">
-        <v>99.94</v>
+        <v>99.87</v>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D77" t="n">
-        <v>0.05</v>
+        <v>0.11</v>
       </c>
       <c r="E77" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="78">
@@ -1758,13 +1758,13 @@
         <v>76</v>
       </c>
       <c r="B78" t="n">
-        <v>99.94</v>
+        <v>99.88</v>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D78" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E78" t="n">
         <v>0</v>
@@ -1775,13 +1775,13 @@
         <v>77</v>
       </c>
       <c r="B79" t="n">
-        <v>99.95</v>
+        <v>99.88</v>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D79" t="n">
-        <v>0.05</v>
+        <v>0.1</v>
       </c>
       <c r="E79" t="n">
         <v>0</v>
@@ -1792,13 +1792,13 @@
         <v>78</v>
       </c>
       <c r="B80" t="n">
-        <v>99.95</v>
+        <v>99.89</v>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D80" t="n">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="E80" t="n">
         <v>0</v>
@@ -1809,13 +1809,13 @@
         <v>79</v>
       </c>
       <c r="B81" t="n">
-        <v>99.95</v>
+        <v>99.89</v>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D81" t="n">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="E81" t="n">
         <v>0</v>
@@ -1826,13 +1826,13 @@
         <v>80</v>
       </c>
       <c r="B82" t="n">
-        <v>99.95999999999999</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="D82" t="n">
-        <v>0.04</v>
+        <v>0.09</v>
       </c>
       <c r="E82" t="n">
         <v>0</v>
@@ -1843,13 +1843,13 @@
         <v>81</v>
       </c>
       <c r="B83" t="n">
-        <v>99.95999999999999</v>
+        <v>99.90000000000001</v>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D83" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="E83" t="n">
         <v>0</v>
@@ -1860,13 +1860,13 @@
         <v>82</v>
       </c>
       <c r="B84" t="n">
-        <v>99.95999999999999</v>
+        <v>99.91</v>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D84" t="n">
-        <v>0.04</v>
+        <v>0.08</v>
       </c>
       <c r="E84" t="n">
         <v>0</v>
@@ -1877,13 +1877,13 @@
         <v>83</v>
       </c>
       <c r="B85" t="n">
-        <v>99.95999999999999</v>
+        <v>99.91</v>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D85" t="n">
-        <v>0.03</v>
+        <v>0.08</v>
       </c>
       <c r="E85" t="n">
         <v>0</v>
@@ -1894,13 +1894,13 @@
         <v>84</v>
       </c>
       <c r="B86" t="n">
-        <v>99.95999999999999</v>
+        <v>99.91</v>
       </c>
       <c r="C86" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D86" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E86" t="n">
         <v>0</v>
@@ -1911,13 +1911,13 @@
         <v>85</v>
       </c>
       <c r="B87" t="n">
-        <v>99.97</v>
+        <v>99.92</v>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D87" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E87" t="n">
         <v>0</v>
@@ -1928,13 +1928,13 @@
         <v>86</v>
       </c>
       <c r="B88" t="n">
-        <v>99.97</v>
+        <v>99.92</v>
       </c>
       <c r="C88" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D88" t="n">
-        <v>0.03</v>
+        <v>0.07000000000000001</v>
       </c>
       <c r="E88" t="n">
         <v>0</v>
@@ -1945,13 +1945,13 @@
         <v>87</v>
       </c>
       <c r="B89" t="n">
-        <v>99.97</v>
+        <v>99.92</v>
       </c>
       <c r="C89" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D89" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="E89" t="n">
         <v>0</v>
@@ -1962,13 +1962,13 @@
         <v>88</v>
       </c>
       <c r="B90" t="n">
-        <v>99.97</v>
+        <v>99.93000000000001</v>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D90" t="n">
-        <v>0.03</v>
+        <v>0.06</v>
       </c>
       <c r="E90" t="n">
         <v>0</v>
@@ -1979,13 +1979,13 @@
         <v>89</v>
       </c>
       <c r="B91" t="n">
-        <v>99.97</v>
+        <v>99.93000000000001</v>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D91" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="E91" t="n">
         <v>0</v>
@@ -1996,13 +1996,13 @@
         <v>90</v>
       </c>
       <c r="B92" t="n">
-        <v>99.97</v>
+        <v>99.93000000000001</v>
       </c>
       <c r="C92" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D92" t="n">
-        <v>0.02</v>
+        <v>0.06</v>
       </c>
       <c r="E92" t="n">
         <v>0</v>
@@ -2013,13 +2013,13 @@
         <v>91</v>
       </c>
       <c r="B93" t="n">
-        <v>99.98</v>
+        <v>99.94</v>
       </c>
       <c r="C93" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D93" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E93" t="n">
         <v>0</v>
@@ -2030,13 +2030,13 @@
         <v>92</v>
       </c>
       <c r="B94" t="n">
-        <v>99.98</v>
+        <v>99.94</v>
       </c>
       <c r="C94" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D94" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E94" t="n">
         <v>0</v>
@@ -2047,13 +2047,13 @@
         <v>93</v>
       </c>
       <c r="B95" t="n">
-        <v>99.98</v>
+        <v>99.94</v>
       </c>
       <c r="C95" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D95" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E95" t="n">
         <v>0</v>
@@ -2064,13 +2064,13 @@
         <v>94</v>
       </c>
       <c r="B96" t="n">
-        <v>99.98</v>
+        <v>99.95</v>
       </c>
       <c r="C96" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D96" t="n">
-        <v>0.02</v>
+        <v>0.05</v>
       </c>
       <c r="E96" t="n">
         <v>0</v>
@@ -2081,13 +2081,13 @@
         <v>95</v>
       </c>
       <c r="B97" t="n">
-        <v>99.98</v>
+        <v>99.95</v>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D97" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E97" t="n">
         <v>0</v>
@@ -2098,13 +2098,13 @@
         <v>96</v>
       </c>
       <c r="B98" t="n">
-        <v>99.98</v>
+        <v>99.95</v>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D98" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E98" t="n">
         <v>0</v>
@@ -2115,13 +2115,13 @@
         <v>97</v>
       </c>
       <c r="B99" t="n">
-        <v>99.98</v>
+        <v>99.95</v>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D99" t="n">
-        <v>0.02</v>
+        <v>0.04</v>
       </c>
       <c r="E99" t="n">
         <v>0</v>
@@ -2132,13 +2132,13 @@
         <v>98</v>
       </c>
       <c r="B100" t="n">
-        <v>99.98</v>
+        <v>99.95</v>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D100" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E100" t="n">
         <v>0</v>
@@ -2149,13 +2149,13 @@
         <v>99</v>
       </c>
       <c r="B101" t="n">
-        <v>99.98</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="C101" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D101" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E101" t="n">
         <v>0</v>
@@ -2166,13 +2166,13 @@
         <v>100</v>
       </c>
       <c r="B102" t="n">
-        <v>99.98999999999999</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D102" t="n">
-        <v>0.01</v>
+        <v>0.04</v>
       </c>
       <c r="E102" t="n">
         <v>0</v>
@@ -2183,13 +2183,13 @@
         <v>101</v>
       </c>
       <c r="B103" t="n">
-        <v>99.98999999999999</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D103" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E103" t="n">
         <v>0</v>
@@ -2200,13 +2200,13 @@
         <v>102</v>
       </c>
       <c r="B104" t="n">
-        <v>99.98999999999999</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="D104" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E104" t="n">
         <v>0</v>
@@ -2217,13 +2217,13 @@
         <v>103</v>
       </c>
       <c r="B105" t="n">
-        <v>99.98999999999999</v>
+        <v>99.95999999999999</v>
       </c>
       <c r="C105" t="n">
         <v>0</v>
       </c>
       <c r="D105" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E105" t="n">
         <v>0</v>
@@ -2234,13 +2234,13 @@
         <v>104</v>
       </c>
       <c r="B106" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C106" t="n">
         <v>0</v>
       </c>
       <c r="D106" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E106" t="n">
         <v>0</v>
@@ -2251,13 +2251,13 @@
         <v>105</v>
       </c>
       <c r="B107" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C107" t="n">
         <v>0</v>
       </c>
       <c r="D107" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E107" t="n">
         <v>0</v>
@@ -2268,13 +2268,13 @@
         <v>106</v>
       </c>
       <c r="B108" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C108" t="n">
         <v>0</v>
       </c>
       <c r="D108" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E108" t="n">
         <v>0</v>
@@ -2285,13 +2285,13 @@
         <v>107</v>
       </c>
       <c r="B109" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C109" t="n">
         <v>0</v>
       </c>
       <c r="D109" t="n">
-        <v>0.01</v>
+        <v>0.03</v>
       </c>
       <c r="E109" t="n">
         <v>0</v>
@@ -2302,13 +2302,13 @@
         <v>108</v>
       </c>
       <c r="B110" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C110" t="n">
         <v>0</v>
       </c>
       <c r="D110" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E110" t="n">
         <v>0</v>
@@ -2319,13 +2319,13 @@
         <v>109</v>
       </c>
       <c r="B111" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C111" t="n">
         <v>0</v>
       </c>
       <c r="D111" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E111" t="n">
         <v>0</v>
@@ -2336,13 +2336,13 @@
         <v>110</v>
       </c>
       <c r="B112" t="n">
-        <v>99.98999999999999</v>
+        <v>99.97</v>
       </c>
       <c r="C112" t="n">
         <v>0</v>
       </c>
       <c r="D112" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E112" t="n">
         <v>0</v>
@@ -2353,16 +2353,16 @@
         <v>111</v>
       </c>
       <c r="B113" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C113" t="n">
         <v>0</v>
       </c>
       <c r="D113" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E113" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="114">
@@ -2370,13 +2370,13 @@
         <v>112</v>
       </c>
       <c r="B114" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C114" t="n">
         <v>0</v>
       </c>
       <c r="D114" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E114" t="n">
         <v>0</v>
@@ -2387,16 +2387,16 @@
         <v>113</v>
       </c>
       <c r="B115" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C115" t="n">
         <v>0</v>
       </c>
       <c r="D115" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E115" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -2404,16 +2404,16 @@
         <v>114</v>
       </c>
       <c r="B116" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C116" t="n">
         <v>0</v>
       </c>
       <c r="D116" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E116" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="117">
@@ -2421,16 +2421,16 @@
         <v>115</v>
       </c>
       <c r="B117" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C117" t="n">
         <v>0</v>
       </c>
       <c r="D117" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E117" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="118">
@@ -2438,16 +2438,16 @@
         <v>116</v>
       </c>
       <c r="B118" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C118" t="n">
         <v>0</v>
       </c>
       <c r="D118" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E118" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -2455,16 +2455,16 @@
         <v>117</v>
       </c>
       <c r="B119" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C119" t="n">
         <v>0</v>
       </c>
       <c r="D119" t="n">
-        <v>0.01</v>
+        <v>0.02</v>
       </c>
       <c r="E119" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -2472,13 +2472,13 @@
         <v>118</v>
       </c>
       <c r="B120" t="n">
-        <v>99.98999999999999</v>
+        <v>99.98</v>
       </c>
       <c r="C120" t="n">
         <v>0</v>
       </c>
       <c r="D120" t="n">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="E120" t="n">
         <v>0</v>
@@ -2489,13 +2489,13 @@
         <v>119</v>
       </c>
       <c r="B121" t="n">
-        <v>100</v>
+        <v>99.98</v>
       </c>
       <c r="C121" t="n">
         <v>0</v>
       </c>
       <c r="D121" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E121" t="n">
         <v>0</v>
@@ -2506,13 +2506,13 @@
         <v>120</v>
       </c>
       <c r="B122" t="n">
-        <v>100</v>
+        <v>99.98</v>
       </c>
       <c r="C122" t="n">
         <v>0</v>
       </c>
       <c r="D122" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E122" t="n">
         <v>0</v>
@@ -2523,13 +2523,13 @@
         <v>121</v>
       </c>
       <c r="B123" t="n">
-        <v>100</v>
+        <v>99.98</v>
       </c>
       <c r="C123" t="n">
         <v>0</v>
       </c>
       <c r="D123" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E123" t="n">
         <v>0</v>
@@ -2540,13 +2540,13 @@
         <v>122</v>
       </c>
       <c r="B124" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C124" t="n">
         <v>0</v>
       </c>
       <c r="D124" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E124" t="n">
         <v>0</v>
@@ -2557,13 +2557,13 @@
         <v>123</v>
       </c>
       <c r="B125" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C125" t="n">
         <v>0</v>
       </c>
       <c r="D125" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E125" t="n">
         <v>0</v>
@@ -2574,13 +2574,13 @@
         <v>124</v>
       </c>
       <c r="B126" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C126" t="n">
         <v>0</v>
       </c>
       <c r="D126" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E126" t="n">
         <v>0</v>
@@ -2591,16 +2591,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C127" t="n">
         <v>0</v>
       </c>
       <c r="D127" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E127" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="128">
@@ -2608,13 +2608,13 @@
         <v>126</v>
       </c>
       <c r="B128" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C128" t="n">
         <v>0</v>
       </c>
       <c r="D128" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E128" t="n">
         <v>0</v>
@@ -2625,16 +2625,16 @@
         <v>127</v>
       </c>
       <c r="B129" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C129" t="n">
         <v>0</v>
       </c>
       <c r="D129" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E129" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="130">
@@ -2642,16 +2642,16 @@
         <v>128</v>
       </c>
       <c r="B130" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C130" t="n">
         <v>0</v>
       </c>
       <c r="D130" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E130" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="131">
@@ -2659,16 +2659,16 @@
         <v>129</v>
       </c>
       <c r="B131" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C131" t="n">
         <v>0</v>
       </c>
       <c r="D131" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E131" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="132">
@@ -2676,16 +2676,16 @@
         <v>130</v>
       </c>
       <c r="B132" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C132" t="n">
         <v>0</v>
       </c>
       <c r="D132" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E132" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="133">
@@ -2693,13 +2693,13 @@
         <v>131</v>
       </c>
       <c r="B133" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C133" t="n">
         <v>0</v>
       </c>
       <c r="D133" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E133" t="n">
         <v>0</v>
@@ -2710,13 +2710,13 @@
         <v>132</v>
       </c>
       <c r="B134" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C134" t="n">
         <v>0</v>
       </c>
       <c r="D134" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E134" t="n">
         <v>0</v>
@@ -2727,13 +2727,13 @@
         <v>133</v>
       </c>
       <c r="B135" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C135" t="n">
         <v>0</v>
       </c>
       <c r="D135" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E135" t="n">
         <v>0</v>
@@ -2744,13 +2744,13 @@
         <v>134</v>
       </c>
       <c r="B136" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C136" t="n">
         <v>0</v>
       </c>
       <c r="D136" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E136" t="n">
         <v>0</v>
@@ -2761,13 +2761,13 @@
         <v>135</v>
       </c>
       <c r="B137" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C137" t="n">
         <v>0</v>
       </c>
       <c r="D137" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E137" t="n">
         <v>0</v>
@@ -2778,13 +2778,13 @@
         <v>136</v>
       </c>
       <c r="B138" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C138" t="n">
         <v>0</v>
       </c>
       <c r="D138" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E138" t="n">
         <v>0</v>
@@ -2795,13 +2795,13 @@
         <v>137</v>
       </c>
       <c r="B139" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C139" t="n">
         <v>0</v>
       </c>
       <c r="D139" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E139" t="n">
         <v>0</v>
@@ -2812,13 +2812,13 @@
         <v>138</v>
       </c>
       <c r="B140" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C140" t="n">
         <v>0</v>
       </c>
       <c r="D140" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E140" t="n">
         <v>0</v>
@@ -2829,13 +2829,13 @@
         <v>139</v>
       </c>
       <c r="B141" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C141" t="n">
         <v>0</v>
       </c>
       <c r="D141" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E141" t="n">
         <v>0</v>
@@ -2846,16 +2846,16 @@
         <v>140</v>
       </c>
       <c r="B142" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C142" t="n">
         <v>0</v>
       </c>
       <c r="D142" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E142" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="143">
@@ -2863,13 +2863,13 @@
         <v>141</v>
       </c>
       <c r="B143" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C143" t="n">
         <v>0</v>
       </c>
       <c r="D143" t="n">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="E143" t="n">
         <v>0</v>
@@ -2880,7 +2880,7 @@
         <v>142</v>
       </c>
       <c r="B144" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C144" t="n">
         <v>0</v>
@@ -2889,7 +2889,7 @@
         <v>0</v>
       </c>
       <c r="E144" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="145">
@@ -2897,7 +2897,7 @@
         <v>143</v>
       </c>
       <c r="B145" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C145" t="n">
         <v>0</v>
@@ -2906,7 +2906,7 @@
         <v>0</v>
       </c>
       <c r="E145" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -2914,7 +2914,7 @@
         <v>144</v>
       </c>
       <c r="B146" t="n">
-        <v>100</v>
+        <v>99.98999999999999</v>
       </c>
       <c r="C146" t="n">
         <v>0</v>
@@ -2923,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="E146" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="147">
@@ -2940,7 +2940,7 @@
         <v>0</v>
       </c>
       <c r="E147" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="148">
@@ -2957,7 +2957,7 @@
         <v>0</v>
       </c>
       <c r="E148" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149">
@@ -3093,7 +3093,7 @@
         <v>0</v>
       </c>
       <c r="E156" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157">
@@ -3110,7 +3110,7 @@
         <v>0</v>
       </c>
       <c r="E157" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="158">
@@ -3161,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="E160" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="161">
@@ -3178,7 +3178,7 @@
         <v>0</v>
       </c>
       <c r="E161" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162">
@@ -3195,7 +3195,7 @@
         <v>0</v>
       </c>
       <c r="E162" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="163">
@@ -3212,7 +3212,7 @@
         <v>0</v>
       </c>
       <c r="E163" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="164">
@@ -3263,7 +3263,7 @@
         <v>0</v>
       </c>
       <c r="E166" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="167">
@@ -3314,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="E169" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="170">
@@ -3382,7 +3382,7 @@
         <v>0</v>
       </c>
       <c r="E173" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="174">
@@ -3416,7 +3416,7 @@
         <v>0</v>
       </c>
       <c r="E175" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="176">
@@ -3433,7 +3433,7 @@
         <v>0</v>
       </c>
       <c r="E176" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="177">
@@ -3518,7 +3518,7 @@
         <v>0</v>
       </c>
       <c r="E181" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="182">
@@ -3535,7 +3535,7 @@
         <v>0</v>
       </c>
       <c r="E182" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="183">
@@ -3603,7 +3603,7 @@
         <v>0</v>
       </c>
       <c r="E186" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187">
@@ -3620,7 +3620,7 @@
         <v>0</v>
       </c>
       <c r="E187" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="188">
@@ -3637,7 +3637,7 @@
         <v>0</v>
       </c>
       <c r="E188" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189">
@@ -3671,7 +3671,7 @@
         <v>0</v>
       </c>
       <c r="E190" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="191">
@@ -3688,7 +3688,7 @@
         <v>0</v>
       </c>
       <c r="E191" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="192">
@@ -3705,7 +3705,7 @@
         <v>0</v>
       </c>
       <c r="E192" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
     </row>
     <row r="193">
@@ -3722,7 +3722,7 @@
         <v>0</v>
       </c>
       <c r="E193" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="194">
@@ -3773,7 +3773,7 @@
         <v>0</v>
       </c>
       <c r="E196" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="197">
@@ -3790,7 +3790,7 @@
         <v>0</v>
       </c>
       <c r="E197" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="198">
@@ -3801,7 +3801,7 @@
         <v>100</v>
       </c>
       <c r="C198" t="n">
-        <v>-0</v>
+        <v>0</v>
       </c>
       <c r="D198" t="n">
         <v>0</v>
@@ -3841,7 +3841,7 @@
         <v>0</v>
       </c>
       <c r="E200" t="n">
-        <v>0</v>
+        <v>-0</v>
       </c>
     </row>
     <row r="201">

</xml_diff>